<commit_message>
Added SARS-CoV-2 analysis, overall Dragen report, strand type
</commit_message>
<xml_diff>
--- a/inputs-sequoia/influent_sequoia_ddpcr.xlsx
+++ b/inputs-sequoia/influent_sequoia_ddpcr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/sequencing-analysis/sequoia/inputs-sequoia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/github/sequoia-dragen/inputs-sequoia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2220AF-783E-C045-A126-C8A0853D34FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BA4C47-B99D-E940-A291-A03E9C1F7B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="500" windowWidth="40980" windowHeight="25360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="500" windowWidth="40980" windowHeight="25360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1810,7 +1810,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1822,29 +1822,29 @@
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
     <col min="11" max="11" width="13.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="14" width="22" style="5" customWidth="1"/>
     <col min="15" max="15" width="21.83203125" style="5" customWidth="1"/>
     <col min="16" max="16" width="21.5" style="23" customWidth="1"/>
     <col min="17" max="17" width="21.83203125" style="24" customWidth="1"/>
-    <col min="18" max="18" width="17.1640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="18.1640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="17" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5" hidden="1" customWidth="1"/>
-    <col min="22" max="23" width="14" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="17.33203125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="13.5" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="13.83203125" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="18" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="13.33203125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="13.1640625" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="13.83203125" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="18" hidden="1" customWidth="1"/>
-    <col min="35" max="36" width="13.1640625" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="13.83203125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" customWidth="1"/>
+    <col min="20" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="12.5" customWidth="1"/>
+    <col min="22" max="23" width="14" customWidth="1"/>
+    <col min="24" max="24" width="17.33203125" customWidth="1"/>
+    <col min="25" max="25" width="13.5" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="13.83203125" customWidth="1"/>
+    <col min="28" max="28" width="18" customWidth="1"/>
+    <col min="29" max="29" width="19.5" customWidth="1"/>
+    <col min="30" max="30" width="17.6640625" customWidth="1"/>
+    <col min="31" max="31" width="13.33203125" customWidth="1"/>
+    <col min="32" max="32" width="13.1640625" customWidth="1"/>
+    <col min="33" max="33" width="13.83203125" customWidth="1"/>
+    <col min="34" max="34" width="18" customWidth="1"/>
+    <col min="35" max="36" width="13.1640625" customWidth="1"/>
+    <col min="37" max="37" width="13.83203125" customWidth="1"/>
     <col min="38" max="38" width="17.33203125" customWidth="1"/>
     <col min="39" max="39" width="16.83203125" customWidth="1"/>
     <col min="40" max="40" width="18" customWidth="1"/>
@@ -21934,12 +21934,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0347FD-7530-7D43-AB52-7DA4F1A53CA5}">
   <dimension ref="A1:AQ12"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.5" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" customWidth="1"/>
     <col min="16" max="16" width="13.1640625" customWidth="1"/>

</xml_diff>